<commit_message>
Upload minutes and backlog changes from 5-11-18
</commit_message>
<xml_diff>
--- a/Management/Backlog and Proposed User Stories.xlsx
+++ b/Management/Backlog and Proposed User Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\game-project-level-6-group-1\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C188E4-25CC-4FF2-9017-842A3967CA42}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AD4EAE-77E4-4245-9987-554D9E58596A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22944" windowHeight="9888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="108">
   <si>
     <t>User Story</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Week 4</t>
-  </si>
-  <si>
     <t>Create a risk assessment for the project</t>
   </si>
   <si>
@@ -336,13 +333,25 @@
   </si>
   <si>
     <t>Implement a "growth tick" that requires the player to water their plant every 6 hours in order to progress it's growth</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Menu flow diagram</t>
+  </si>
+  <si>
+    <t>Sprint 3 (not set as task)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -420,8 +429,23 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,6 +468,11 @@
       <patternFill patternType="solid">
         <fgColor indexed="22"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -545,10 +574,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -600,13 +630,17 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -952,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K140"/>
+  <dimension ref="A1:K141"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -963,7 +997,7 @@
     <col min="2" max="2" width="91.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="99.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="69.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.33203125" customWidth="1"/>
@@ -1011,45 +1045,53 @@
         <v>6</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>7</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="15"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
+        <v>7</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
+        <v>79</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
-      <c r="C8" s="16" t="s">
-        <v>96</v>
+      <c r="C8" s="30" t="s">
+        <v>95</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -1059,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
@@ -1067,52 +1109,52 @@
     </row>
     <row r="10" spans="1:8">
       <c r="C10" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="C11" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="C12" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="C13" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8">
       <c r="C15" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="C16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="C17" s="29" t="s">
-        <v>101</v>
+      <c r="C17" s="28" t="s">
+        <v>100</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
@@ -1123,7 +1165,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -1133,7 +1175,7 @@
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
       <c r="C19" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
@@ -1142,7 +1184,7 @@
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
@@ -1151,7 +1193,7 @@
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
@@ -1161,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="18"/>
       <c r="D22" s="18"/>
@@ -1171,16 +1213,20 @@
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
+        <v>14</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
@@ -1190,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
@@ -1200,16 +1246,20 @@
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
       <c r="C26" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
+        <v>16</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
@@ -1219,7 +1269,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
@@ -1229,16 +1279,20 @@
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
       <c r="C29" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
+        <v>99</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
       <c r="C30" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>6</v>
@@ -1250,7 +1304,7 @@
         <v>1</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
@@ -1260,17 +1314,21 @@
       <c r="A32" s="20"/>
       <c r="B32" s="20"/>
       <c r="C32" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
+        <v>19</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="18">
         <v>1</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
@@ -1280,7 +1338,7 @@
       <c r="A34" s="20"/>
       <c r="B34" s="20"/>
       <c r="C34" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D34" s="20"/>
       <c r="E34" s="20"/>
@@ -1289,7 +1347,7 @@
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="20" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D35" s="20"/>
       <c r="E35" s="20"/>
@@ -1298,7 +1356,7 @@
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
@@ -1308,7 +1366,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -1319,7 +1377,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
@@ -1329,7 +1387,7 @@
       <c r="A39" s="20"/>
       <c r="B39" s="20"/>
       <c r="C39" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
@@ -1338,235 +1396,247 @@
       <c r="A40" s="20"/>
       <c r="B40" s="20"/>
       <c r="C40" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
+        <v>106</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="C41" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D41" s="20"/>
       <c r="E41" s="20"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="18">
+      <c r="A42" s="20"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="18">
         <v>2</v>
       </c>
-      <c r="B42" s="25" t="s">
+      <c r="B43" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="18">
+        <v>2</v>
+      </c>
+      <c r="B45" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="18">
-        <v>2</v>
-      </c>
-      <c r="B44" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="20"/>
       <c r="B46" s="20"/>
       <c r="C46" s="20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D46" s="20"/>
       <c r="E46" s="20"/>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="18">
+      <c r="A47" s="20"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="18">
         <v>2</v>
       </c>
-      <c r="B47" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="C48" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
+      <c r="B48" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
     </row>
     <row r="49" spans="1:11">
       <c r="C49" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="18">
+      <c r="C50" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="18">
         <v>2</v>
       </c>
-      <c r="B50" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="18"/>
-      <c r="D50" s="18"/>
-      <c r="E50" s="18"/>
-    </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="20"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
+      <c r="B51" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="20"/>
       <c r="B52" s="20"/>
       <c r="C52" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
+        <v>89</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="18">
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="18">
         <v>2</v>
       </c>
-      <c r="B53" s="18" t="s">
+      <c r="B54" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="20"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="18">
+        <v>2</v>
+      </c>
+      <c r="B56" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D54" s="20"/>
-      <c r="E54" s="20"/>
-    </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="18">
-        <v>2</v>
-      </c>
-      <c r="B55" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-    </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="20"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="20"/>
       <c r="B57" s="20"/>
       <c r="C57" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D57" s="20"/>
       <c r="E57" s="20"/>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="18">
+      <c r="A58" s="20"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="18">
         <v>2</v>
       </c>
-      <c r="B58" s="18" t="s">
+      <c r="B59" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="J59" s="22"/>
+      <c r="K59" s="22"/>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="C60" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C58" s="18"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18"/>
-      <c r="J58" s="22"/>
-      <c r="K58" s="22"/>
-    </row>
-    <row r="59" spans="1:11">
-      <c r="C59" s="20" t="s">
+      <c r="D60" s="21"/>
+      <c r="E60" s="20"/>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="18">
+        <v>3</v>
+      </c>
+      <c r="B61" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D59" s="21"/>
-      <c r="E59" s="20"/>
-    </row>
-    <row r="60" spans="1:11">
-      <c r="A60" s="18">
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="20"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="18">
         <v>3</v>
       </c>
-      <c r="B60" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-    </row>
-    <row r="61" spans="1:11">
-      <c r="A61" s="20"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20" t="s">
+      <c r="B63" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-    </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="18">
-        <v>3</v>
-      </c>
-      <c r="B62" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-    </row>
-    <row r="63" spans="1:11">
-      <c r="A63" s="20"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
     </row>
     <row r="64" spans="1:11">
       <c r="A64" s="20"/>
       <c r="B64" s="20"/>
       <c r="C64" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D64" s="20"/>
       <c r="E64" s="20"/>
@@ -1575,7 +1645,7 @@
       <c r="A65" s="20"/>
       <c r="B65" s="20"/>
       <c r="C65" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D65" s="20"/>
       <c r="E65" s="20"/>
@@ -1584,7 +1654,7 @@
       <c r="A66" s="20"/>
       <c r="B66" s="20"/>
       <c r="C66" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D66" s="20"/>
       <c r="E66" s="20"/>
@@ -1593,143 +1663,145 @@
       <c r="A67" s="20"/>
       <c r="B67" s="20"/>
       <c r="C67" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D67" s="20"/>
       <c r="E67" s="20"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="18">
-        <v>3</v>
-      </c>
-      <c r="B68" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C68" s="18"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
+      <c r="A68" s="20"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D68" s="20"/>
+      <c r="E68" s="20"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="18">
         <v>3</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C69" s="18"/>
       <c r="D69" s="18"/>
       <c r="E69" s="18"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="20"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D70" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E70" s="20" t="s">
-        <v>97</v>
-      </c>
+      <c r="A70" s="18">
+        <v>3</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C70" s="18"/>
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="20"/>
       <c r="B71" s="20"/>
       <c r="C71" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D71" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="20"/>
       <c r="B72" s="20"/>
       <c r="C72" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D72" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E72" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="20"/>
       <c r="B73" s="20"/>
       <c r="C73" s="20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D73" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E73" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="20"/>
       <c r="B74" s="20"/>
       <c r="C74" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D74" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E74" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="20"/>
       <c r="B75" s="20"/>
       <c r="C75" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D75" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E75" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="20"/>
       <c r="B76" s="20"/>
       <c r="C76" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D76" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E76" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="20"/>
       <c r="B77" s="20"/>
       <c r="C77" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D77" s="20" t="s">
         <v>6</v>
       </c>
       <c r="E77" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="20"/>
       <c r="B78" s="20"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="20"/>
+      <c r="C78" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" s="20" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="20"/>
@@ -2053,26 +2125,33 @@
       <c r="D124" s="20"/>
       <c r="E124" s="20"/>
     </row>
-    <row r="128" spans="1:5">
-      <c r="C128" s="19"/>
-    </row>
-    <row r="139" spans="1:5">
-      <c r="A139" s="17">
-        <v>3</v>
-      </c>
-      <c r="B139" s="17"/>
-      <c r="C139" s="17"/>
-      <c r="D139" s="17"/>
-      <c r="E139" s="17"/>
+    <row r="125" spans="1:5">
+      <c r="A125" s="20"/>
+      <c r="B125" s="20"/>
+      <c r="C125" s="20"/>
+      <c r="D125" s="20"/>
+      <c r="E125" s="20"/>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="C129" s="19"/>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="17">
         <v>3</v>
       </c>
-      <c r="B140" s="23"/>
+      <c r="B140" s="17"/>
       <c r="C140" s="17"/>
       <c r="D140" s="17"/>
       <c r="E140" s="17"/>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" s="17">
+        <v>3</v>
+      </c>
+      <c r="B141" s="23"/>
+      <c r="C141" s="17"/>
+      <c r="D141" s="17"/>
+      <c r="E141" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2085,7 +2164,7 @@
   <dimension ref="B3:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2098,66 +2177,66 @@
   <sheetData>
     <row r="3" spans="2:16">
       <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="2:16">
       <c r="B4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="P4" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="2:16">
       <c r="B5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="P5" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="2:16">
       <c r="B6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="P6" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="P6" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:16">
       <c r="B7" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -2170,132 +2249,132 @@
     </row>
     <row r="8" spans="2:16">
       <c r="B8" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:16">
       <c r="B9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
     </row>
     <row r="10" spans="2:16">
       <c r="B10" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="27"/>
-      <c r="M10" s="27"/>
-      <c r="N10" s="27"/>
+        <v>59</v>
+      </c>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
     </row>
     <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="2:16">
       <c r="B12" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="2:16">
       <c r="B13" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="2:16">
       <c r="B14" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="2:16">
       <c r="B15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="2:16">
       <c r="B16" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4">
+      <c r="B17" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="2:4">
-      <c r="B17" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated backlog and risk assessment
Updated backlog and risk assessment reviewed during weekly sprint meeting
</commit_message>
<xml_diff>
--- a/Management/Backlog and Proposed User Stories.xlsx
+++ b/Management/Backlog and Proposed User Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\game-project-level-6-group-1\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D2EED0-6289-4837-9848-FD5F6098874F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF225D09-3FDC-4B30-9744-6B13C452F0C2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22944" windowHeight="9888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="111">
   <si>
     <t>User Story</t>
   </si>
@@ -329,9 +329,6 @@
     <t>Implement a system in Unity that allows the player to collect "stars" from fully grown objects</t>
   </si>
   <si>
-    <t xml:space="preserve">Create a rarity table that dictates how much energy/stars can be earned for each type of object </t>
-  </si>
-  <si>
     <t>Implement a "growth tick" that requires the player to water their plant every 6 hours in order to progress it's growth</t>
   </si>
   <si>
@@ -354,6 +351,9 @@
   </si>
   <si>
     <t>Create a countdown timer that displays time until object is fully grown</t>
+  </si>
+  <si>
+    <t>Create a spreadsheet, that details how much energy can be earned from different objects</t>
   </si>
 </sst>
 </file>
@@ -366,13 +366,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -435,11 +428,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -453,8 +441,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +484,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -583,73 +595,81 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -998,7 +1018,7 @@
   <dimension ref="A1:K142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1048,63 +1068,63 @@
     <row r="4" spans="1:8">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="29" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>104</v>
+      <c r="D5" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="15"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="16" t="s">
+      <c r="D6" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="29" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="16" t="s">
-        <v>104</v>
+      <c r="D7" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="17">
@@ -1118,80 +1138,97 @@
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>108</v>
+      <c r="D10" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>107</v>
       </c>
       <c r="H10" s="24" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="30" t="s">
         <v>80</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>107</v>
       </c>
       <c r="H11" s="24" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="30" t="s">
         <v>85</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>107</v>
       </c>
       <c r="H12" s="24" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="31" t="s">
         <v>86</v>
       </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="C14" t="s">
+      <c r="C14" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D14" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="C15" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="C15" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" t="s">
-        <v>109</v>
-      </c>
-      <c r="E15" t="s">
-        <v>108</v>
+      <c r="E15" s="30" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="C16" t="s">
+      <c r="C16" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" t="s">
-        <v>108</v>
+      <c r="D16" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="D17" t="s">
-        <v>6</v>
+      <c r="D17" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1208,11 +1245,15 @@
     <row r="19" spans="1:5">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
+      <c r="D19" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="20"/>
@@ -1246,14 +1287,14 @@
     <row r="23" spans="1:5">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>104</v>
+      <c r="D23" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1279,13 +1320,13 @@
     <row r="26" spans="1:5">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="20" t="s">
+      <c r="D26" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="30" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1293,7 +1334,7 @@
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="20"/>
@@ -1302,7 +1343,7 @@
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
@@ -1321,26 +1362,28 @@
     <row r="30" spans="1:5">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="D30" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>107</v>
+      <c r="D30" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="20"/>
+      <c r="D31" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="18">
@@ -1356,13 +1399,13 @@
     <row r="33" spans="1:5">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="20" t="s">
+      <c r="D33" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="30" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1380,26 +1423,30 @@
     <row r="35" spans="1:5">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
-      <c r="C36" s="20" t="s">
+      <c r="C36" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
+      <c r="D36" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D37" s="20"/>
       <c r="E37" s="20"/>
@@ -1438,14 +1485,14 @@
     <row r="41" spans="1:5">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
-      <c r="C41" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="D41" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" s="20" t="s">
+      <c r="C41" s="30" t="s">
         <v>105</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1552,27 +1599,27 @@
     <row r="53" spans="1:11">
       <c r="A53" s="20"/>
       <c r="B53" s="20"/>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="D53" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="20" t="s">
-        <v>105</v>
+      <c r="D53" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="D54" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="20" t="s">
-        <v>105</v>
+      <c r="D54" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -1745,104 +1792,104 @@
     <row r="72" spans="1:5">
       <c r="A72" s="20"/>
       <c r="B72" s="20"/>
-      <c r="C72" s="20" t="s">
+      <c r="C72" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D72" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E72" s="20" t="s">
+      <c r="D72" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="20"/>
       <c r="B73" s="20"/>
-      <c r="C73" s="20" t="s">
+      <c r="C73" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D73" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E73" s="20" t="s">
+      <c r="D73" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="20"/>
       <c r="B74" s="20"/>
-      <c r="C74" s="20" t="s">
+      <c r="C74" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D74" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74" s="20" t="s">
+      <c r="D74" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="20"/>
       <c r="B75" s="20"/>
-      <c r="C75" s="20" t="s">
+      <c r="C75" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D75" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E75" s="20" t="s">
+      <c r="D75" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="20"/>
       <c r="B76" s="20"/>
-      <c r="C76" s="20" t="s">
+      <c r="C76" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="D76" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E76" s="20" t="s">
+      <c r="D76" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="20"/>
       <c r="B77" s="20"/>
-      <c r="C77" s="20" t="s">
+      <c r="C77" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="D77" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E77" s="20" t="s">
+      <c r="D77" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="20"/>
       <c r="B78" s="20"/>
-      <c r="C78" s="20" t="s">
+      <c r="C78" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="D78" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E78" s="20" t="s">
+      <c r="D78" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="20"/>
       <c r="B79" s="20"/>
-      <c r="C79" s="20" t="s">
+      <c r="C79" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D79" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E79" s="20" t="s">
+      <c r="D79" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="30" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2207,7 +2254,7 @@
   <dimension ref="B3:P17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2311,17 +2358,17 @@
       <c r="D9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
     </row>
     <row r="10" spans="2:16">
       <c r="B10" s="2" t="s">
@@ -2333,15 +2380,15 @@
       <c r="D10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
     </row>
     <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">
@@ -2395,7 +2442,7 @@
         <v>59</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:16">
@@ -2410,7 +2457,7 @@
       </c>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="26" t="s">
         <v>91</v>
       </c>
       <c r="C17" s="2" t="s">

</xml_diff>

<commit_message>
updated backlog to reflect recent sprint
</commit_message>
<xml_diff>
--- a/Management/Backlog and Proposed User Stories.xlsx
+++ b/Management/Backlog and Proposed User Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\game-project-level-6-group-1\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF225D09-3FDC-4B30-9744-6B13C452F0C2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457A35D5-D065-4F46-ABC5-669F2AA30EBA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22944" windowHeight="9888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="112">
   <si>
     <t>User Story</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>Create a spreadsheet, that details how much energy can be earned from different objects</t>
+  </si>
+  <si>
+    <t>Sprint 6</t>
   </si>
 </sst>
 </file>
@@ -654,9 +657,6 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -664,6 +664,9 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1017,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1068,52 +1071,52 @@
     <row r="4" spans="1:8">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="29" t="s">
+      <c r="D4" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="28" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="29" t="s">
+      <c r="D5" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="28" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="15"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="29" t="s">
+      <c r="D6" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="28" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="29" t="s">
+      <c r="D7" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="28" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1123,8 +1126,8 @@
       <c r="C8" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="17">
@@ -1138,13 +1141,13 @@
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="29" t="s">
+      <c r="D10" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="28" t="s">
         <v>107</v>
       </c>
       <c r="H10" s="24" t="s">
@@ -1152,13 +1155,13 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="D11" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="29" t="s">
+      <c r="D11" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="28" t="s">
         <v>107</v>
       </c>
       <c r="H11" s="24" t="s">
@@ -1166,13 +1169,13 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="29" t="s">
+      <c r="D12" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="28" t="s">
         <v>107</v>
       </c>
       <c r="H12" s="24" t="s">
@@ -1180,54 +1183,54 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="30" t="s">
+      <c r="D14" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="29" t="s">
         <v>107</v>
       </c>
       <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="29" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="30" t="s">
+      <c r="D16" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="29" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="D17" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="30" t="s">
+      <c r="D17" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="29" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1245,24 +1248,28 @@
     <row r="19" spans="1:5">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="30" t="s">
+      <c r="D19" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="29" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
+      <c r="D20" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="29" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="20"/>
@@ -1287,13 +1294,13 @@
     <row r="23" spans="1:5">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="30" t="s">
+      <c r="D23" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="29" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1320,24 +1327,24 @@
     <row r="26" spans="1:5">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
-      <c r="C26" s="30" t="s">
+      <c r="C26" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="30" t="s">
+      <c r="D26" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="29" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="20"/>
@@ -1362,26 +1369,26 @@
     <row r="30" spans="1:5">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="D30" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="30" t="s">
+      <c r="D30" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="29" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="30" t="s">
+      <c r="D31" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="29" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1399,13 +1406,13 @@
     <row r="33" spans="1:5">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="30" t="s">
+      <c r="D33" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="29" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1423,33 +1430,37 @@
     <row r="35" spans="1:5">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
-      <c r="C35" s="31" t="s">
+      <c r="C35" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
-      <c r="C36" s="30" t="s">
+      <c r="C36" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="D36" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" s="30" t="s">
+      <c r="D36" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="29" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
-      <c r="C37" s="20" t="s">
+      <c r="C37" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
+      <c r="D37" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="18">
@@ -1485,13 +1496,13 @@
     <row r="41" spans="1:5">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
-      <c r="C41" s="30" t="s">
+      <c r="C41" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="D41" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" s="30" t="s">
+      <c r="D41" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="29" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1599,26 +1610,26 @@
     <row r="53" spans="1:11">
       <c r="A53" s="20"/>
       <c r="B53" s="20"/>
-      <c r="C53" s="30" t="s">
+      <c r="C53" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="D53" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="30" t="s">
+      <c r="D53" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="29" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
-      <c r="C54" s="30" t="s">
+      <c r="C54" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="D54" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="30" t="s">
+      <c r="D54" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="29" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1792,104 +1803,104 @@
     <row r="72" spans="1:5">
       <c r="A72" s="20"/>
       <c r="B72" s="20"/>
-      <c r="C72" s="30" t="s">
+      <c r="C72" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D72" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E72" s="30" t="s">
+      <c r="D72" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" s="29" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="20"/>
       <c r="B73" s="20"/>
-      <c r="C73" s="30" t="s">
+      <c r="C73" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D73" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E73" s="30" t="s">
+      <c r="D73" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="29" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="20"/>
       <c r="B74" s="20"/>
-      <c r="C74" s="30" t="s">
+      <c r="C74" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D74" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74" s="30" t="s">
+      <c r="D74" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="29" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="20"/>
       <c r="B75" s="20"/>
-      <c r="C75" s="30" t="s">
+      <c r="C75" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D75" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E75" s="30" t="s">
+      <c r="D75" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="29" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="20"/>
       <c r="B76" s="20"/>
-      <c r="C76" s="30" t="s">
+      <c r="C76" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="D76" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E76" s="30" t="s">
+      <c r="D76" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" s="29" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="20"/>
       <c r="B77" s="20"/>
-      <c r="C77" s="30" t="s">
+      <c r="C77" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D77" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E77" s="30" t="s">
+      <c r="D77" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="29" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="20"/>
       <c r="B78" s="20"/>
-      <c r="C78" s="30" t="s">
+      <c r="C78" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D78" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E78" s="30" t="s">
+      <c r="D78" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" s="29" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="20"/>
       <c r="B79" s="20"/>
-      <c r="C79" s="30" t="s">
+      <c r="C79" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="D79" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E79" s="30" t="s">
+      <c r="D79" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="29" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2358,17 +2369,17 @@
       <c r="D9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="28" t="s">
+      <c r="F9" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
     </row>
     <row r="10" spans="2:16">
       <c r="B10" s="2" t="s">
@@ -2380,15 +2391,15 @@
       <c r="D10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
     </row>
     <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">

</xml_diff>

<commit_message>
update backlog and risk assessment for current week
</commit_message>
<xml_diff>
--- a/Management/Backlog and Proposed User Stories.xlsx
+++ b/Management/Backlog and Proposed User Stories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\game-project-level-6-group-1\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457A35D5-D065-4F46-ABC5-669F2AA30EBA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C5CF23-845A-43C5-A1BB-C9B8E519FEF5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22944" windowHeight="9888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="119">
   <si>
     <t>User Story</t>
   </si>
@@ -308,9 +308,6 @@
     <t>Create a consumer profile/psychographic</t>
   </si>
   <si>
-    <t>Project timeline?</t>
-  </si>
-  <si>
     <t>Sprint 2</t>
   </si>
   <si>
@@ -350,20 +347,44 @@
     <t xml:space="preserve">Done </t>
   </si>
   <si>
-    <t>Create a countdown timer that displays time until object is fully grown</t>
-  </si>
-  <si>
     <t>Create a spreadsheet, that details how much energy can be earned from different objects</t>
   </si>
   <si>
     <t>Sprint 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Progress </t>
+  </si>
+  <si>
+    <t>Broken</t>
+  </si>
+  <si>
+    <t>Project timeline</t>
+  </si>
+  <si>
+    <t>As a UI element, create a countdown timer that displays time until object is fully grown</t>
+  </si>
+  <si>
+    <t>WK9</t>
+  </si>
+  <si>
+    <t>WK8</t>
+  </si>
+  <si>
+    <t>WK10</t>
+  </si>
+  <si>
+    <t>WK11</t>
+  </si>
+  <si>
+    <t>WK12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,14 +458,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -500,7 +513,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -597,14 +610,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -654,19 +676,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -675,7 +699,43 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFCC0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1020,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1071,60 +1131,60 @@
     <row r="4" spans="1:8">
       <c r="A4" s="15"/>
       <c r="B4" s="16"/>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>96</v>
+      <c r="D4" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>103</v>
+      <c r="D5" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="15"/>
       <c r="B6" s="16"/>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>96</v>
+      <c r="D6" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>103</v>
+      <c r="D7" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
-      <c r="C8" s="27" t="s">
-        <v>95</v>
+      <c r="C8" s="31" t="s">
+        <v>112</v>
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
@@ -1141,100 +1201,110 @@
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>107</v>
+      <c r="D10" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>106</v>
       </c>
       <c r="H10" s="24" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D11" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>107</v>
+      <c r="D11" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>106</v>
       </c>
       <c r="H11" s="24" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>107</v>
+      <c r="D12" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>106</v>
       </c>
       <c r="H12" s="24" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
+      <c r="D13" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="29" t="s">
+      <c r="D14" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="C15" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="H14" s="24"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="C15" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>107</v>
+      <c r="E15" s="28" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="D16" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="C17" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="D16" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="C17" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="H17" s="29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="17">
         <v>1</v>
       </c>
@@ -1244,43 +1314,46 @@
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="H18" s="30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="D19" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="D20" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="18">
         <v>1</v>
       </c>
@@ -1291,29 +1364,29 @@
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:8">
       <c r="A23" s="20"/>
       <c r="B23" s="20"/>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="D23" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" s="18">
         <v>1</v>
       </c>
@@ -1324,38 +1397,42 @@
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:8">
       <c r="A26" s="20"/>
       <c r="B26" s="20"/>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="D26" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
-      <c r="C27" s="30" t="s">
+      <c r="C27" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-    </row>
-    <row r="28" spans="1:5">
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
-      <c r="C28" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="C28" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="30"/>
+      <c r="E28" s="30"/>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="18">
         <v>1</v>
       </c>
@@ -1366,33 +1443,33 @@
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:8">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
-      <c r="C30" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="C30" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
-      <c r="C31" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="C31" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" s="18">
         <v>1</v>
       </c>
@@ -1406,14 +1483,14 @@
     <row r="33" spans="1:5">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E33" s="29" t="s">
-        <v>96</v>
+      <c r="D33" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1430,36 +1507,40 @@
     <row r="35" spans="1:5">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
-      <c r="C35" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
+      <c r="C35" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
-      <c r="C36" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="D36" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" s="29" t="s">
-        <v>107</v>
+      <c r="C36" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
-      <c r="C37" s="29" t="s">
-        <v>110</v>
-      </c>
-      <c r="D37" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="29" t="s">
-        <v>111</v>
+      <c r="C37" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1496,14 +1577,14 @@
     <row r="41" spans="1:5">
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
-      <c r="C41" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" s="29" t="s">
+      <c r="C41" s="28" t="s">
         <v>104</v>
+      </c>
+      <c r="D41" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1610,27 +1691,27 @@
     <row r="53" spans="1:11">
       <c r="A53" s="20"/>
       <c r="B53" s="20"/>
-      <c r="C53" s="29" t="s">
+      <c r="C53" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="D53" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="29" t="s">
-        <v>104</v>
+      <c r="D53" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="28" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
-      <c r="C54" s="29" t="s">
+      <c r="C54" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="D54" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="29" t="s">
-        <v>104</v>
+      <c r="D54" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="28" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -1667,11 +1748,11 @@
     <row r="58" spans="1:11">
       <c r="A58" s="20"/>
       <c r="B58" s="20"/>
-      <c r="C58" s="20" t="s">
+      <c r="C58" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="20"/>
@@ -1803,105 +1884,105 @@
     <row r="72" spans="1:5">
       <c r="A72" s="20"/>
       <c r="B72" s="20"/>
-      <c r="C72" s="29" t="s">
+      <c r="C72" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="D72" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E72" s="29" t="s">
-        <v>96</v>
+      <c r="D72" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" s="28" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="20"/>
       <c r="B73" s="20"/>
-      <c r="C73" s="29" t="s">
+      <c r="C73" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D73" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E73" s="29" t="s">
-        <v>96</v>
+      <c r="D73" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="28" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="20"/>
       <c r="B74" s="20"/>
-      <c r="C74" s="29" t="s">
+      <c r="C74" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D74" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74" s="29" t="s">
-        <v>96</v>
+      <c r="D74" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="28" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="20"/>
       <c r="B75" s="20"/>
-      <c r="C75" s="29" t="s">
+      <c r="C75" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D75" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E75" s="29" t="s">
-        <v>96</v>
+      <c r="D75" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="28" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="20"/>
       <c r="B76" s="20"/>
-      <c r="C76" s="29" t="s">
+      <c r="C76" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="D76" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E76" s="29" t="s">
-        <v>96</v>
+      <c r="D76" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" s="28" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="20"/>
       <c r="B77" s="20"/>
-      <c r="C77" s="29" t="s">
+      <c r="C77" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D77" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E77" s="29" t="s">
-        <v>96</v>
+      <c r="D77" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="28" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="20"/>
       <c r="B78" s="20"/>
-      <c r="C78" s="29" t="s">
+      <c r="C78" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="D78" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E78" s="29" t="s">
-        <v>96</v>
+      <c r="D78" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" s="28" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="20"/>
       <c r="B79" s="20"/>
-      <c r="C79" s="29" t="s">
+      <c r="C79" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D79" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E79" s="29" t="s">
-        <v>96</v>
+      <c r="D79" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="28" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2262,10 +2343,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B3:P17"/>
+  <dimension ref="B2:P22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2273,9 +2354,26 @@
     <col min="2" max="2" width="48.21875" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:16">
+      <c r="D2" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>118</v>
+      </c>
+    </row>
     <row r="3" spans="2:16">
       <c r="B3" s="1" t="s">
         <v>54</v>
@@ -2286,6 +2384,12 @@
       <c r="D3" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="2:16">
       <c r="B4" s="2" t="s">
@@ -2297,6 +2401,12 @@
       <c r="D4" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
       <c r="P4" s="5" t="s">
         <v>58</v>
       </c>
@@ -2311,6 +2421,12 @@
       <c r="D5" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
       <c r="P5" s="5" t="s">
         <v>59</v>
       </c>
@@ -2325,6 +2441,12 @@
       <c r="D6" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="E6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
       <c r="P6" s="5" t="s">
         <v>62</v>
       </c>
@@ -2337,11 +2459,14 @@
         <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -2358,6 +2483,12 @@
       <c r="D8" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="E8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="2:16">
       <c r="B9" s="2" t="s">
@@ -2369,17 +2500,12 @@
       <c r="D9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
+      <c r="E9" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="2:16">
       <c r="B10" s="2" t="s">
@@ -2391,15 +2517,12 @@
       <c r="D10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
+      <c r="E10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:16">
       <c r="B11" s="2" t="s">
@@ -2411,6 +2534,12 @@
       <c r="D11" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="E11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="2:16">
       <c r="B12" s="2" t="s">
@@ -2422,6 +2551,12 @@
       <c r="D12" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="E12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="2:16">
       <c r="B13" s="2" t="s">
@@ -2433,6 +2568,12 @@
       <c r="D13" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="E13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="2:16">
       <c r="B14" s="2" t="s">
@@ -2444,6 +2585,12 @@
       <c r="D14" s="2" t="s">
         <v>59</v>
       </c>
+      <c r="E14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="2:16">
       <c r="B15" s="2" t="s">
@@ -2455,6 +2602,12 @@
       <c r="D15" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="E15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" spans="2:16">
       <c r="B16" s="2" t="s">
@@ -2466,8 +2619,14 @@
       <c r="D16" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="2:4">
+      <c r="E16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="2:10">
       <c r="B17" s="26" t="s">
         <v>91</v>
       </c>
@@ -2477,24 +2636,65 @@
       <c r="D17" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="E17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F9:N10"/>
+    <mergeCell ref="B21:J22"/>
   </mergeCells>
   <conditionalFormatting sqref="C4:D17">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="equal">
       <formula>$P$5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E17">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>$P$5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:D17" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:E17" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$P$4:$P$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Latest project version & Discord Log for first half of Week 10
</commit_message>
<xml_diff>
--- a/Management/Backlog and Proposed User Stories.xlsx
+++ b/Management/Backlog and Proposed User Stories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\game-project-level-6-group-1\Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2kXswitX\Documents\GitHub\game-project-level-6-group-1\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C5CF23-845A-43C5-A1BB-C9B8E519FEF5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AE32F0-8255-49E2-BFB6-7B9CE4A64364}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22944" windowHeight="9888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="22950" windowHeight="9885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -686,11 +686,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1080,20 +1080,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
-    <col min="2" max="2" width="91.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="108.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="91.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="108.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="69.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" customWidth="1"/>
+    <col min="8" max="8" width="69.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1426,11 +1426,11 @@
     <row r="28" spans="1:8">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="18">
@@ -2345,16 +2345,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:P22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="48.21875" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" customWidth="1"/>
+    <col min="2" max="2" width="48.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16">
@@ -2464,9 +2464,9 @@
       <c r="E7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -2644,28 +2644,28 @@
       <c r="H17" s="2"/>
     </row>
     <row r="21" spans="2:10">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
     </row>
     <row r="22" spans="2:10">
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Revert "Update backlog documentation"
This reverts commit dfe8f2d9fccf7447d3017aa4ad4069f60545ec9c.
</commit_message>
<xml_diff>
--- a/Management/Backlog and Proposed User Stories.xlsx
+++ b/Management/Backlog and Proposed User Stories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\game-project-level-6-group-1\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACE3B59-14F5-4CE6-968A-DC02377E550A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C5CF23-845A-43C5-A1BB-C9B8E519FEF5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22944" windowHeight="9888" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22944" windowHeight="9888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="119">
   <si>
     <t>User Story</t>
   </si>
@@ -686,11 +686,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1080,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K142"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1671,11 +1671,11 @@
       <c r="E50" s="20"/>
     </row>
     <row r="51" spans="1:11">
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
     </row>
     <row r="52" spans="1:11">
       <c r="A52" s="18">
@@ -2345,8 +2345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:P22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2387,9 +2387,7 @@
       <c r="E3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>56</v>
-      </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
@@ -2466,9 +2464,9 @@
       <c r="E7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -2646,28 +2644,28 @@
       <c r="H17" s="2"/>
     </row>
     <row r="21" spans="2:10">
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
     </row>
     <row r="22" spans="2:10">
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
uploaded document for iterated sorting/tending mechanics
</commit_message>
<xml_diff>
--- a/Management/Backlog and Proposed User Stories.xlsx
+++ b/Management/Backlog and Proposed User Stories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2kXswitX\Documents\GitHub\game-project-level-6-group-1\Management\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\game-project-level-6-group-1\Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AE32F0-8255-49E2-BFB6-7B9CE4A64364}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71BB2CE-47DC-43A9-B92F-FCA3F956E35A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="22950" windowHeight="9885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="22956" windowHeight="9888" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="126">
   <si>
     <t>User Story</t>
   </si>
@@ -269,9 +269,6 @@
     <t>Create concept art for the layout of the sorting screen</t>
   </si>
   <si>
-    <t>As a player I want to be able to progress to unlock new sorting categories and their corresponding items</t>
-  </si>
-  <si>
     <t>Come up with the two initial sorting categories</t>
   </si>
   <si>
@@ -378,6 +375,30 @@
   </si>
   <si>
     <t>WK12</t>
+  </si>
+  <si>
+    <t>Menu mock up</t>
+  </si>
+  <si>
+    <t>In Unity, create a pop-up that displays the planet name at the beginning of each play session</t>
+  </si>
+  <si>
+    <t>Should this be priority 2 now? Seasons provide optimum times for players to gather and perform certain activities</t>
+  </si>
+  <si>
+    <t>"As a user I want to be able to tend to my planet in different ways"</t>
+  </si>
+  <si>
+    <t>"As a user I want to be able to nurture my planet"</t>
+  </si>
+  <si>
+    <t>As a player I want to be able to unlock new sorting categories and their corresponding items</t>
+  </si>
+  <si>
+    <t>As a player I want to be feel a sense of progression in the game</t>
+  </si>
+  <si>
+    <t>Determine the length of play for the game</t>
   </si>
 </sst>
 </file>
@@ -626,7 +647,7 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -692,6 +713,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1078,22 +1101,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K142"/>
+  <dimension ref="A1:K147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="91.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="108.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="91.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="69.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" customWidth="1"/>
+    <col min="8" max="8" width="80.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1138,20 +1161,20 @@
         <v>6</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="15"/>
       <c r="B5" s="16"/>
       <c r="C5" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1164,7 +1187,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -1177,14 +1200,14 @@
         <v>6</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="15"/>
       <c r="B8" s="16"/>
       <c r="C8" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D8" s="31"/>
       <c r="E8" s="31"/>
@@ -1208,7 +1231,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H10" s="24" t="s">
         <v>76</v>
@@ -1222,7 +1245,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H11" s="24" t="s">
         <v>77</v>
@@ -1230,13 +1253,13 @@
     </row>
     <row r="12" spans="1:8">
       <c r="C12" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H12" s="24" t="s">
         <v>78</v>
@@ -1244,13 +1267,13 @@
     </row>
     <row r="13" spans="1:8">
       <c r="C13" s="28" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D13" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1261,30 +1284,30 @@
         <v>6</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8">
       <c r="C15" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="C16" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D16" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H16" s="28" t="s">
         <v>6</v>
@@ -1292,16 +1315,16 @@
     </row>
     <row r="17" spans="1:8">
       <c r="C17" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D17" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1315,7 +1338,7 @@
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="H18" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1328,7 +1351,7 @@
         <v>6</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1341,14 +1364,14 @@
         <v>6</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="20"/>
       <c r="B21" s="20"/>
       <c r="C21" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D21" s="29"/>
       <c r="E21" s="29"/>
@@ -1374,14 +1397,14 @@
         <v>6</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="20"/>
       <c r="B24" s="20"/>
       <c r="C24" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="29"/>
@@ -1407,27 +1430,27 @@
         <v>6</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="C27" s="28" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D27" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="C28" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
@@ -1447,26 +1470,26 @@
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
       <c r="C30" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D30" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
       <c r="C31" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D31" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1490,7 +1513,7 @@
         <v>6</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1498,7 +1521,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
@@ -1508,39 +1531,39 @@
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
       <c r="C35" s="28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D35" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
       <c r="C36" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D36" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="C37" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" s="28" t="s">
         <v>108</v>
-      </c>
-      <c r="D37" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" s="28" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1548,477 +1571,498 @@
         <v>2</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
+        <v>124</v>
+      </c>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="18">
-        <v>2</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="20"/>
+      <c r="C39" t="s">
+        <v>125</v>
+      </c>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="20"/>
       <c r="B40" s="20"/>
-      <c r="C40" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="D41" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E41" s="28" t="s">
-        <v>103</v>
-      </c>
+      <c r="A41" s="18">
+        <v>2</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
+      <c r="A42" s="18">
+        <v>2</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="C43" s="20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D43" s="20"/>
       <c r="E43" s="20"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="18">
-        <v>2</v>
-      </c>
-      <c r="B44" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="20"/>
       <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
+      <c r="C45" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D45" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="28" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="18">
-        <v>2</v>
-      </c>
-      <c r="B46" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
+      <c r="A46" s="20"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="20"/>
       <c r="B47" s="20"/>
       <c r="C47" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D47" s="20"/>
       <c r="E47" s="20"/>
     </row>
     <row r="48" spans="1:5">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-    </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="18">
+      <c r="A48" s="18">
         <v>2</v>
       </c>
-      <c r="B49" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-    </row>
-    <row r="50" spans="1:11">
-      <c r="C50" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-    </row>
-    <row r="51" spans="1:11">
+      <c r="B48" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="20"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="18">
+        <v>2</v>
+      </c>
+      <c r="B50" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C50" s="18"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="20"/>
+      <c r="B51" s="20"/>
       <c r="C51" s="20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D51" s="20"/>
       <c r="E51" s="20"/>
     </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="18">
+    <row r="52" spans="1:5">
+      <c r="A52" s="20"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="18">
         <v>2</v>
       </c>
-      <c r="B52" s="18" t="s">
+      <c r="B53" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="C54" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="C55" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="18">
+        <v>2</v>
+      </c>
+      <c r="B56" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
-    </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="20"/>
-      <c r="B53" s="20"/>
-      <c r="C53" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="D53" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E53" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="D54" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E54" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="18">
-        <v>2</v>
-      </c>
-      <c r="B55" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C55" s="18"/>
-      <c r="D55" s="18"/>
-      <c r="E55" s="18"/>
-    </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="20"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20" t="s">
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="20"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-    </row>
-    <row r="57" spans="1:11">
-      <c r="A57" s="18">
-        <v>2</v>
-      </c>
-      <c r="B57" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="C57" s="18"/>
-      <c r="D57" s="18"/>
-      <c r="E57" s="18"/>
-    </row>
-    <row r="58" spans="1:11">
+      <c r="D57" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="20"/>
       <c r="B58" s="20"/>
-      <c r="C58" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-    </row>
-    <row r="59" spans="1:11">
+      <c r="C58" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="28" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="20"/>
       <c r="B59" s="20"/>
-      <c r="C59" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-    </row>
-    <row r="60" spans="1:11">
+      <c r="C59" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" s="18">
         <v>2</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C60" s="18"/>
       <c r="D60" s="18"/>
       <c r="E60" s="18"/>
-      <c r="J60" s="22"/>
-      <c r="K60" s="22"/>
-    </row>
-    <row r="61" spans="1:11">
-      <c r="C61" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D61" s="21"/>
-      <c r="E61" s="20"/>
-    </row>
-    <row r="62" spans="1:11">
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="20"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:5">
       <c r="A63" s="20"/>
       <c r="B63" s="20"/>
-      <c r="C63" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-    </row>
-    <row r="64" spans="1:11">
-      <c r="A64" s="18">
+      <c r="C63" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="20"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="18">
+        <v>2</v>
+      </c>
+      <c r="B65" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="J65" s="22"/>
+      <c r="K65" s="22"/>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="C66" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D66" s="21"/>
+      <c r="E66" s="20"/>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="18">
         <v>3</v>
       </c>
-      <c r="B64" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C64" s="18"/>
-      <c r="D64" s="18"/>
-      <c r="E64" s="18"/>
-    </row>
-    <row r="65" spans="1:5">
-      <c r="A65" s="20"/>
-      <c r="B65" s="20"/>
-      <c r="C65" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
-    </row>
-    <row r="66" spans="1:5">
-      <c r="A66" s="20"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D66" s="20"/>
-      <c r="E66" s="20"/>
-    </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="20"/>
-      <c r="B67" s="20"/>
-      <c r="C67" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="B67" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C67" s="18"/>
+      <c r="D67" s="18"/>
+      <c r="E67" s="18"/>
+    </row>
+    <row r="68" spans="1:11">
       <c r="A68" s="20"/>
       <c r="B68" s="20"/>
       <c r="C68" s="20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D68" s="20"/>
       <c r="E68" s="20"/>
     </row>
-    <row r="69" spans="1:5">
-      <c r="A69" s="20"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" s="18">
+    <row r="69" spans="1:11">
+      <c r="A69" s="18">
         <v>3</v>
       </c>
-      <c r="B70" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" s="18">
-        <v>3</v>
-      </c>
-      <c r="B71" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="B69" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="20"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="20"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
+    </row>
+    <row r="72" spans="1:11">
       <c r="A72" s="20"/>
       <c r="B72" s="20"/>
-      <c r="C72" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="D72" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E72" s="28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="C72" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D72" s="20"/>
+      <c r="E72" s="20"/>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" s="20"/>
       <c r="B73" s="20"/>
-      <c r="C73" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D73" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E73" s="28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="C73" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" s="20"/>
       <c r="B74" s="20"/>
-      <c r="C74" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="D74" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74" s="28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="A75" s="20"/>
-      <c r="B75" s="20"/>
-      <c r="C75" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D75" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E75" s="28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="A76" s="20"/>
-      <c r="B76" s="20"/>
-      <c r="C76" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D76" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E76" s="28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="C74" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D74" s="20"/>
+      <c r="E74" s="20"/>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="18">
+        <v>3</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="18">
+        <v>3</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="H76" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" s="20"/>
       <c r="B77" s="20"/>
       <c r="C77" s="28" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D77" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E77" s="28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
+        <v>94</v>
+      </c>
+      <c r="H77" s="28" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="20"/>
       <c r="B78" s="20"/>
       <c r="C78" s="28" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D78" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E78" s="28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
+        <v>94</v>
+      </c>
+      <c r="H78" s="28" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" s="20"/>
       <c r="B79" s="20"/>
       <c r="C79" s="28" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D79" s="28" t="s">
         <v>6</v>
       </c>
       <c r="E79" s="28" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80" s="20"/>
       <c r="B80" s="20"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="20"/>
+      <c r="C80" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D80" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" s="28" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="20"/>
       <c r="B81" s="20"/>
-      <c r="C81" s="20"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="20"/>
+      <c r="C81" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D81" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" s="28" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="20"/>
       <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="20"/>
+      <c r="C82" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D82" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" s="28" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="20"/>
       <c r="B83" s="20"/>
-      <c r="C83" s="20"/>
-      <c r="D83" s="20"/>
-      <c r="E83" s="20"/>
+      <c r="C83" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D83" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" s="28" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="20"/>
       <c r="B84" s="20"/>
-      <c r="C84" s="20"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="20"/>
+      <c r="C84" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D84" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" s="28" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="20"/>
@@ -2314,26 +2358,61 @@
       <c r="D126" s="20"/>
       <c r="E126" s="20"/>
     </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="20"/>
+      <c r="B127" s="20"/>
+      <c r="C127" s="20"/>
+      <c r="D127" s="20"/>
+      <c r="E127" s="20"/>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="20"/>
+      <c r="B128" s="20"/>
+      <c r="C128" s="20"/>
+      <c r="D128" s="20"/>
+      <c r="E128" s="20"/>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" s="20"/>
+      <c r="B129" s="20"/>
+      <c r="C129" s="20"/>
+      <c r="D129" s="20"/>
+      <c r="E129" s="20"/>
+    </row>
     <row r="130" spans="1:5">
-      <c r="C130" s="19"/>
-    </row>
-    <row r="141" spans="1:5">
-      <c r="A141" s="17">
+      <c r="A130" s="20"/>
+      <c r="B130" s="20"/>
+      <c r="C130" s="20"/>
+      <c r="D130" s="20"/>
+      <c r="E130" s="20"/>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" s="20"/>
+      <c r="B131" s="20"/>
+      <c r="C131" s="20"/>
+      <c r="D131" s="20"/>
+      <c r="E131" s="20"/>
+    </row>
+    <row r="135" spans="1:5">
+      <c r="C135" s="19"/>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="A146" s="17">
         <v>3</v>
       </c>
-      <c r="B141" s="17"/>
-      <c r="C141" s="17"/>
-      <c r="D141" s="17"/>
-      <c r="E141" s="17"/>
-    </row>
-    <row r="142" spans="1:5">
-      <c r="A142" s="17">
+      <c r="B146" s="17"/>
+      <c r="C146" s="17"/>
+      <c r="D146" s="17"/>
+      <c r="E146" s="17"/>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="A147" s="17">
         <v>3</v>
       </c>
-      <c r="B142" s="23"/>
-      <c r="C142" s="17"/>
-      <c r="D142" s="17"/>
-      <c r="E142" s="17"/>
+      <c r="B147" s="23"/>
+      <c r="C147" s="17"/>
+      <c r="D147" s="17"/>
+      <c r="E147" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2345,33 +2424,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:P22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="48.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:16">
       <c r="D2" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="32" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="32" t="s">
-        <v>114</v>
-      </c>
-      <c r="F2" s="32" t="s">
+      <c r="G2" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="H2" s="32" t="s">
         <v>117</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="3" spans="2:16">
@@ -2387,7 +2466,9 @@
       <c r="E3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
@@ -2404,7 +2485,9 @@
       <c r="E4" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="P4" s="5" t="s">
@@ -2424,7 +2507,9 @@
       <c r="E5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="P5" s="5" t="s">
@@ -2444,7 +2529,9 @@
       <c r="E6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="P6" s="5" t="s">
@@ -2464,7 +2551,9 @@
       <c r="E7" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F7" s="33"/>
+      <c r="F7" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="G7" s="33"/>
       <c r="H7" s="33"/>
       <c r="I7" s="4"/>
@@ -2486,7 +2575,9 @@
       <c r="E8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
@@ -2503,7 +2594,9 @@
       <c r="E9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
@@ -2520,7 +2613,9 @@
       <c r="E10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
@@ -2537,7 +2632,9 @@
       <c r="E11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
@@ -2554,7 +2651,9 @@
       <c r="E12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
@@ -2571,7 +2670,9 @@
       <c r="E13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
@@ -2586,9 +2687,11 @@
         <v>59</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -2605,7 +2708,9 @@
       <c r="E15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
@@ -2622,13 +2727,15 @@
       <c r="E16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="2:10">
       <c r="B17" s="26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>59</v>
@@ -2639,7 +2746,9 @@
       <c r="E17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
@@ -2682,7 +2791,7 @@
       <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4:E17">
+  <conditionalFormatting sqref="E4:F17">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
@@ -2694,7 +2803,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:E17" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:F17" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>$P$4:$P$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>